<commit_message>
cohort_id added and code 125 to no_name to avoid duplicate kanc cohort, again
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
@@ -18,6 +18,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>JU</author>
+  </authors>
+  <commentList>
+    <comment ref="D26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Kanc was repeated</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4471,7 +4494,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4493,6 +4516,10 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13544,494 +13571,494 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>1278</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1279</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>1280</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="9" t="n">
         <v>101</v>
       </c>
-      <c r="C2" s="9" t="b">
+      <c r="C2" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>1281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="9" t="n">
         <v>102</v>
       </c>
-      <c r="C3" s="9" t="b">
+      <c r="C3" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>1282</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="9" t="n">
         <v>103</v>
       </c>
-      <c r="C4" s="9" t="b">
+      <c r="C4" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>1283</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="9" t="n">
         <v>104</v>
       </c>
-      <c r="C5" s="9" t="b">
+      <c r="C5" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>1284</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="9" t="n">
         <v>105</v>
       </c>
-      <c r="C6" s="9" t="b">
+      <c r="C6" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>1285</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>106</v>
       </c>
-      <c r="C7" s="9" t="b">
+      <c r="C7" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>1286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>107</v>
       </c>
-      <c r="C8" s="9" t="b">
+      <c r="C8" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>1287</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="9" t="n">
         <v>108</v>
       </c>
-      <c r="C9" s="9" t="b">
+      <c r="C9" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>1288</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="9" t="n">
         <v>109</v>
       </c>
-      <c r="C10" s="9" t="b">
+      <c r="C10" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <v>110</v>
       </c>
-      <c r="C11" s="9" t="b">
+      <c r="C11" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>1290</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="9" t="n">
         <v>111</v>
       </c>
-      <c r="C12" s="9" t="b">
+      <c r="C12" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>1291</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>112</v>
       </c>
-      <c r="C13" s="9" t="b">
+      <c r="C13" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>1292</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="9" t="n">
         <v>113</v>
       </c>
-      <c r="C14" s="9" t="b">
+      <c r="C14" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>1293</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="9" t="n">
         <v>114</v>
       </c>
-      <c r="C15" s="9" t="b">
+      <c r="C15" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>1294</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="9" t="n">
         <v>115</v>
       </c>
-      <c r="C16" s="9" t="b">
+      <c r="C16" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>1295</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>116</v>
       </c>
-      <c r="C17" s="9" t="b">
+      <c r="C17" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>1296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="9" t="n">
         <v>117</v>
       </c>
-      <c r="C18" s="9" t="b">
+      <c r="C18" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>1297</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="9" t="n">
         <v>118</v>
       </c>
-      <c r="C19" s="9" t="b">
+      <c r="C19" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>1298</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="9" t="n">
         <v>119</v>
       </c>
-      <c r="C20" s="9" t="b">
+      <c r="C20" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>1299</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="C21" s="9" t="b">
+      <c r="C21" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="9" t="n">
         <v>121</v>
       </c>
-      <c r="C22" s="9" t="b">
+      <c r="C22" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>1301</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="9" t="n">
         <v>122</v>
       </c>
-      <c r="C23" s="9" t="b">
+      <c r="C23" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>1302</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="9" t="n">
         <v>123</v>
       </c>
-      <c r="C24" s="9" t="b">
+      <c r="C24" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>1303</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="9" t="n">
         <v>124</v>
       </c>
-      <c r="C25" s="9" t="b">
+      <c r="C25" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>1304</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B26" s="9" t="n">
         <v>125</v>
       </c>
-      <c r="C26" s="9" t="b">
+      <c r="C26" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>1305</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="9" t="n">
         <v>126</v>
       </c>
-      <c r="C27" s="9" t="b">
+      <c r="C27" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>1306</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="9" t="n">
         <v>127</v>
       </c>
-      <c r="C28" s="9" t="b">
+      <c r="C28" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="9" t="n">
         <v>128</v>
       </c>
-      <c r="C29" s="9" t="b">
+      <c r="C29" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9" t="s">
         <v>1308</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="9" t="n">
         <v>129</v>
       </c>
-      <c r="C30" s="9" t="b">
+      <c r="C30" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>1309</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="9" t="n">
         <v>130</v>
       </c>
-      <c r="C31" s="9" t="b">
+      <c r="C31" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="9" t="n">
         <v>131</v>
       </c>
-      <c r="C32" s="9" t="b">
+      <c r="C32" s="10" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>1311</v>
       </c>
     </row>
@@ -14043,5 +14070,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced cohort_id no_name with helix and removed column name table
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
@@ -20,31 +20,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author>JU</author>
-  </authors>
-  <commentList>
-    <comment ref="D26" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Kanc was repeated</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="1311">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -3880,9 +3857,6 @@
     <t xml:space="preserve">Limit of detection of newborn  2-MPA at birth</t>
   </si>
   <si>
-    <t xml:space="preserve">table</t>
-  </si>
-  <si>
     <t xml:space="preserve">variable</t>
   </si>
   <si>
@@ -3961,7 +3935,7 @@
     <t xml:space="preserve">environage </t>
   </si>
   <si>
-    <t xml:space="preserve">no_name</t>
+    <t xml:space="preserve">helix</t>
   </si>
   <si>
     <t xml:space="preserve">pelagie</t>
@@ -3990,7 +3964,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4138,13 +4112,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC9211E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -4210,7 +4177,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFC9211E"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -4494,7 +4461,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4536,10 +4503,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4645,7 +4608,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF1A1A1A"/>
@@ -4655,17 +4618,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D634"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="26"/>
@@ -13548,14 +13511,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B634" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B634" type="list">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13564,36 +13527,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>1278</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1279</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>1280</v>
-      </c>
-      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -13604,12 +13564,12 @@
       <c r="B2" s="9" t="n">
         <v>101</v>
       </c>
-      <c r="C2" s="10" t="b">
+      <c r="C2" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13619,12 +13579,12 @@
       <c r="B3" s="9" t="n">
         <v>102</v>
       </c>
-      <c r="C3" s="10" t="b">
+      <c r="C3" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13634,12 +13594,12 @@
       <c r="B4" s="9" t="n">
         <v>103</v>
       </c>
-      <c r="C4" s="10" t="b">
+      <c r="C4" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13649,12 +13609,12 @@
       <c r="B5" s="9" t="n">
         <v>104</v>
       </c>
-      <c r="C5" s="10" t="b">
+      <c r="C5" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13664,12 +13624,12 @@
       <c r="B6" s="9" t="n">
         <v>105</v>
       </c>
-      <c r="C6" s="10" t="b">
+      <c r="C6" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13679,12 +13639,12 @@
       <c r="B7" s="9" t="n">
         <v>106</v>
       </c>
-      <c r="C7" s="10" t="b">
+      <c r="C7" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13694,12 +13654,12 @@
       <c r="B8" s="9" t="n">
         <v>107</v>
       </c>
-      <c r="C8" s="10" t="b">
+      <c r="C8" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13709,12 +13669,12 @@
       <c r="B9" s="9" t="n">
         <v>108</v>
       </c>
-      <c r="C9" s="10" t="b">
+      <c r="C9" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13724,12 +13684,12 @@
       <c r="B10" s="9" t="n">
         <v>109</v>
       </c>
-      <c r="C10" s="10" t="b">
+      <c r="C10" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13739,12 +13699,12 @@
       <c r="B11" s="9" t="n">
         <v>110</v>
       </c>
-      <c r="C11" s="10" t="b">
+      <c r="C11" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13754,12 +13714,12 @@
       <c r="B12" s="9" t="n">
         <v>111</v>
       </c>
-      <c r="C12" s="10" t="b">
+      <c r="C12" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13769,12 +13729,12 @@
       <c r="B13" s="9" t="n">
         <v>112</v>
       </c>
-      <c r="C13" s="10" t="b">
+      <c r="C13" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13784,12 +13744,12 @@
       <c r="B14" s="9" t="n">
         <v>113</v>
       </c>
-      <c r="C14" s="10" t="b">
+      <c r="C14" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13799,12 +13759,12 @@
       <c r="B15" s="9" t="n">
         <v>114</v>
       </c>
-      <c r="C15" s="10" t="b">
+      <c r="C15" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13814,12 +13774,12 @@
       <c r="B16" s="9" t="n">
         <v>115</v>
       </c>
-      <c r="C16" s="10" t="b">
+      <c r="C16" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13829,12 +13789,12 @@
       <c r="B17" s="9" t="n">
         <v>116</v>
       </c>
-      <c r="C17" s="10" t="b">
+      <c r="C17" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13844,12 +13804,12 @@
       <c r="B18" s="9" t="n">
         <v>117</v>
       </c>
-      <c r="C18" s="10" t="b">
+      <c r="C18" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13859,12 +13819,12 @@
       <c r="B19" s="9" t="n">
         <v>118</v>
       </c>
-      <c r="C19" s="10" t="b">
+      <c r="C19" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13874,12 +13834,12 @@
       <c r="B20" s="9" t="n">
         <v>119</v>
       </c>
-      <c r="C20" s="10" t="b">
+      <c r="C20" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13889,12 +13849,12 @@
       <c r="B21" s="9" t="n">
         <v>120</v>
       </c>
-      <c r="C21" s="10" t="b">
+      <c r="C21" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13904,12 +13864,12 @@
       <c r="B22" s="9" t="n">
         <v>121</v>
       </c>
-      <c r="C22" s="10" t="b">
+      <c r="C22" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13919,12 +13879,12 @@
       <c r="B23" s="9" t="n">
         <v>122</v>
       </c>
-      <c r="C23" s="10" t="b">
+      <c r="C23" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13934,12 +13894,12 @@
       <c r="B24" s="9" t="n">
         <v>123</v>
       </c>
-      <c r="C24" s="10" t="b">
+      <c r="C24" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13949,27 +13909,27 @@
       <c r="B25" s="9" t="n">
         <v>124</v>
       </c>
-      <c r="C25" s="10" t="b">
+      <c r="C25" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>125</v>
       </c>
-      <c r="C26" s="10" t="b">
+      <c r="C26" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>1305</v>
+      <c r="D26" s="9" t="s">
+        <v>1304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13979,12 +13939,12 @@
       <c r="B27" s="9" t="n">
         <v>126</v>
       </c>
-      <c r="C27" s="10" t="b">
+      <c r="C27" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13994,12 +13954,12 @@
       <c r="B28" s="9" t="n">
         <v>127</v>
       </c>
-      <c r="C28" s="10" t="b">
+      <c r="C28" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14009,12 +13969,12 @@
       <c r="B29" s="9" t="n">
         <v>128</v>
       </c>
-      <c r="C29" s="10" t="b">
+      <c r="C29" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14024,12 +13984,12 @@
       <c r="B30" s="9" t="n">
         <v>129</v>
       </c>
-      <c r="C30" s="10" t="b">
+      <c r="C30" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14039,12 +13999,12 @@
       <c r="B31" s="9" t="n">
         <v>130</v>
       </c>
-      <c r="C31" s="10" t="b">
+      <c r="C31" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14054,22 +14014,21 @@
       <c r="B32" s="9" t="n">
         <v>131</v>
       </c>
-      <c r="C32" s="10" t="b">
+      <c r="C32" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed column missing to isMissing in 1_1_non_rep.xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
@@ -3860,7 +3860,7 @@
     <t xml:space="preserve">variable</t>
   </si>
   <si>
-    <t xml:space="preserve">missing</t>
+    <t xml:space="preserve">isMissing</t>
   </si>
   <si>
     <t xml:space="preserve">genr</t>
@@ -13534,10 +13534,10 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="26"/>

</xml_diff>

<commit_message>
isMissing =FALSE() to string false for chemicals_ath 1_1_non_rep.xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="1311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="1312">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -3861,6 +3861,9 @@
   </si>
   <si>
     <t xml:space="preserve">isMissing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">genr</t>
@@ -3962,7 +3965,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -4461,7 +4464,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4490,7 +4493,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="18" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="18" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13534,492 +13545,462 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="26"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
         <v>1278</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>1279</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="C2" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="D2" s="11" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="C3" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="C4" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="C4" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="C5" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>1283</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="C5" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="11" t="n">
         <v>105</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="C6" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="11" t="n">
         <v>106</v>
       </c>
-      <c r="C7" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="C7" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="11" t="n">
         <v>107</v>
       </c>
-      <c r="C8" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="C8" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="11" t="n">
         <v>108</v>
       </c>
-      <c r="C9" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="C9" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="11" t="n">
         <v>109</v>
       </c>
-      <c r="C10" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="C10" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="11" t="n">
         <v>110</v>
       </c>
-      <c r="C11" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>1289</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="C11" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="11" t="n">
         <v>111</v>
       </c>
-      <c r="C12" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="11" t="n">
         <v>112</v>
       </c>
-      <c r="C13" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="C13" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="11" t="n">
         <v>113</v>
       </c>
-      <c r="C14" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="C14" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="11" t="n">
         <v>114</v>
       </c>
-      <c r="C15" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="C15" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="11" t="n">
         <v>115</v>
       </c>
-      <c r="C16" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="C16" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="11" t="n">
         <v>116</v>
       </c>
-      <c r="C17" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="C17" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="11" t="n">
         <v>117</v>
       </c>
-      <c r="C18" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="C18" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="11" t="n">
         <v>118</v>
       </c>
-      <c r="C19" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="C19" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="11" t="n">
         <v>119</v>
       </c>
-      <c r="C20" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="C20" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="11" t="n">
         <v>120</v>
       </c>
-      <c r="C21" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="C21" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="11" t="n">
         <v>121</v>
       </c>
-      <c r="C22" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="C22" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="9" t="n">
+      <c r="B23" s="11" t="n">
         <v>122</v>
       </c>
-      <c r="C23" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
+      <c r="C23" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="11" t="n">
         <v>123</v>
       </c>
-      <c r="C24" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+      <c r="C24" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="11" t="n">
         <v>124</v>
       </c>
-      <c r="C25" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>1303</v>
+      <c r="C25" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>1304</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="11" t="n">
         <v>125</v>
       </c>
-      <c r="C26" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+      <c r="C26" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="9" t="n">
+      <c r="B27" s="11" t="n">
         <v>126</v>
       </c>
-      <c r="C27" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+      <c r="C27" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="9" t="n">
+      <c r="B28" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="C28" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+      <c r="C28" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="9" t="n">
+      <c r="B29" s="11" t="n">
         <v>128</v>
       </c>
-      <c r="C29" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+      <c r="C29" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="9" t="n">
+      <c r="B30" s="11" t="n">
         <v>129</v>
       </c>
-      <c r="C30" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+      <c r="C30" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="9" t="n">
+      <c r="B31" s="11" t="n">
         <v>130</v>
       </c>
-      <c r="C31" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
+      <c r="C31" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="9" t="n">
+      <c r="B32" s="11" t="n">
         <v>131</v>
       </c>
-      <c r="C32" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>1310</v>
+      <c r="C32" s="12" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>1311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chemicals_ath 1_1_non_rep.xlsx column isMissing to 0 or 1
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_1/1_1_non_rep.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="1311">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -3861,9 +3861,6 @@
   </si>
   <si>
     <t xml:space="preserve">isMissing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">genr</t>
@@ -3963,9 +3960,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -4493,7 +4489,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4501,7 +4497,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="18" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="18" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4513,7 +4509,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13545,10 +13541,10 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="26"/>
@@ -13576,11 +13572,11 @@
       <c r="B2" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>1280</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13590,11 +13586,11 @@
       <c r="B3" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>1280</v>
+      <c r="C3" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13604,11 +13600,11 @@
       <c r="B4" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>1280</v>
+      <c r="C4" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13618,11 +13614,11 @@
       <c r="B5" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>1280</v>
+      <c r="C5" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13632,11 +13628,11 @@
       <c r="B6" s="11" t="n">
         <v>105</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>1280</v>
+      <c r="C6" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13646,11 +13642,11 @@
       <c r="B7" s="11" t="n">
         <v>106</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>1280</v>
+      <c r="C7" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13660,11 +13656,11 @@
       <c r="B8" s="11" t="n">
         <v>107</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>1280</v>
+      <c r="C8" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13674,11 +13670,11 @@
       <c r="B9" s="11" t="n">
         <v>108</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>1280</v>
+      <c r="C9" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13688,11 +13684,11 @@
       <c r="B10" s="11" t="n">
         <v>109</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>1280</v>
+      <c r="C10" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13702,11 +13698,11 @@
       <c r="B11" s="11" t="n">
         <v>110</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>1280</v>
+      <c r="C11" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13716,11 +13712,11 @@
       <c r="B12" s="11" t="n">
         <v>111</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>1280</v>
+      <c r="C12" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13730,11 +13726,11 @@
       <c r="B13" s="11" t="n">
         <v>112</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>1280</v>
+      <c r="C13" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13744,11 +13740,11 @@
       <c r="B14" s="11" t="n">
         <v>113</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>1280</v>
+      <c r="C14" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13758,11 +13754,11 @@
       <c r="B15" s="11" t="n">
         <v>114</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>1280</v>
+      <c r="C15" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13772,11 +13768,11 @@
       <c r="B16" s="11" t="n">
         <v>115</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>1280</v>
+      <c r="C16" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13786,11 +13782,11 @@
       <c r="B17" s="11" t="n">
         <v>116</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>1280</v>
+      <c r="C17" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13800,11 +13796,11 @@
       <c r="B18" s="11" t="n">
         <v>117</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>1280</v>
+      <c r="C18" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13814,11 +13810,11 @@
       <c r="B19" s="11" t="n">
         <v>118</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>1280</v>
+      <c r="C19" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13828,11 +13824,11 @@
       <c r="B20" s="11" t="n">
         <v>119</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>1280</v>
+      <c r="C20" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13842,11 +13838,11 @@
       <c r="B21" s="11" t="n">
         <v>120</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>1280</v>
+      <c r="C21" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13856,11 +13852,11 @@
       <c r="B22" s="11" t="n">
         <v>121</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>1280</v>
+      <c r="C22" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13870,11 +13866,11 @@
       <c r="B23" s="11" t="n">
         <v>122</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>1280</v>
+      <c r="C23" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13884,11 +13880,11 @@
       <c r="B24" s="11" t="n">
         <v>123</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>1280</v>
+      <c r="C24" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13898,11 +13894,11 @@
       <c r="B25" s="11" t="n">
         <v>124</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>1280</v>
+      <c r="C25" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13912,11 +13908,11 @@
       <c r="B26" s="11" t="n">
         <v>125</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>1280</v>
+      <c r="C26" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13926,11 +13922,11 @@
       <c r="B27" s="11" t="n">
         <v>126</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>1280</v>
+      <c r="C27" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13940,11 +13936,11 @@
       <c r="B28" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>1280</v>
+      <c r="C28" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13954,11 +13950,11 @@
       <c r="B29" s="11" t="n">
         <v>128</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>1280</v>
+      <c r="C29" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13968,11 +13964,11 @@
       <c r="B30" s="11" t="n">
         <v>129</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>1280</v>
+      <c r="C30" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13982,11 +13978,11 @@
       <c r="B31" s="11" t="n">
         <v>130</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>1280</v>
+      <c r="C31" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13996,11 +13992,11 @@
       <c r="B32" s="11" t="n">
         <v>131</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>1280</v>
+      <c r="C32" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>